<commit_message>
Update constact-summary forms to use new template
</commit_message>
<xml_diff>
--- a/contact-summary/forms/app/with_contact_summary.xlsx
+++ b/contact-summary/forms/app/with_contact_summary.xlsx
@@ -11,7 +11,7 @@
     <sheet name="survey" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="settings" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -20,8 +20,195 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author>Unknown Author</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Determines what kinds of values are allowed and how the field is displayed. For certain types, further customization is possible using the appearance and parameters columns.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF0000FF"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">https://docs.getodk.org/form-question-types/
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Variable name. It may not contain spaces and must start with a letter or underscore. You should use a short, descriptive name and can use underscores to separate words. For example: date_of_birth.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">The user-visible question text for the field. For example: "When was ${first_name} born?" This text can optionally reference other fields or be styled using subsets of Markdown and HTML.
+Can be translated.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">One or more modifiers that determine how the question will be displayed.
+These can be specific to the field type.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">An expression that will be evaluated to determine the value of the field.
+⚠️ Expressions may be re-evaluated at any time. 
+To limit when expressions are evaluated, for example to specify dynamic defaults use the once() function. 
+https://docs.getodk.org/form-logic/#when-expressions-are-evaluated</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">The number of instances of a repeat to create. Can be a fixed value or a 
+dynamic expression.
+https://docs.getodk.org/form-logic/#fixed-repeat-count</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Can include a human-friendly note to describe the row. This will be ignored by all ODK tools.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author>Unknown Author</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">The title that will be displayed to anyone who uses this form.
+https://docs.getodk.org/xlsform/#the-settings-sheet</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">The unique ID that identifies this form to tools that use it. It may not contain spaces and must start with a letter or underscore. You should use a short, descriptive name and can use underscores to separate words. 
+For example: bench_inventory_2021
+You can change the form_title as much as you would like but if you change the form_id, it will be considered a different form definition.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">The unique version code that identifies the current state of the form. A common convention is to use a format like yyyymmddrr. For example, 2017021501 is the 1st revision from Feb 15th, 2017.
+By default, this template uses a formula to create a date-based version that will update automatically.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Set to ‘pages’ to indicate that groups with the `field-list` appearance represent separate form pages (and all other questions will be shown on their own page). </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Custom namespaces supported in the form.  `cht` must be included here to use the custom `instance::cht` columns on the survey sheet.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="53">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -29,7 +216,10 @@
     <t xml:space="preserve">name</t>
   </si>
   <si>
-    <t xml:space="preserve">label::en</t>
+    <t xml:space="preserve">label::English (en)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">appearance</t>
   </si>
   <si>
     <t xml:space="preserve">calculation</t>
@@ -38,7 +228,7 @@
     <t xml:space="preserve">repeat_count</t>
   </si>
   <si>
-    <t xml:space="preserve">appearance</t>
+    <t xml:space="preserve">note</t>
   </si>
   <si>
     <t xml:space="preserve">begin_group</t>
@@ -74,9 +264,6 @@
     <t xml:space="preserve">instance(‘contact-summary’)/context/favorite_chw/referrals</t>
   </si>
   <si>
-    <t xml:space="preserve">note</t>
-  </si>
-  <si>
     <t xml:space="preserve">favorite_note</t>
   </si>
   <si>
@@ -155,7 +342,7 @@
     <t xml:space="preserve">end_group</t>
   </si>
   <si>
-    <t xml:space="preserve">title</t>
+    <t xml:space="preserve">form_title</t>
   </si>
   <si>
     <t xml:space="preserve">form_id</t>
@@ -167,10 +354,7 @@
     <t xml:space="preserve">style</t>
   </si>
   <si>
-    <t xml:space="preserve">path</t>
-  </si>
-  <si>
-    <t xml:space="preserve">default_language</t>
+    <t xml:space="preserve">namespaces</t>
   </si>
   <si>
     <t xml:space="preserve">Contact Summary Test</t>
@@ -182,26 +366,23 @@
     <t xml:space="preserve">pages</t>
   </si>
   <si>
-    <t xml:space="preserve">data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">en</t>
+    <t xml:space="preserve">cht=https://communityhealthtoolkit.org</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="mm/dd/yy\ hh:mm\ AM/PM"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -220,41 +401,46 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="Cambria"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
-      <name val="Cambria"/>
-      <family val="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAFD095"/>
+        <bgColor rgb="FFCCCCCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -262,8 +448,71 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair">
+        <color rgb="FF999999"/>
+      </left>
+      <right style="hair">
+        <color rgb="FF999999"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair">
+        <color rgb="FF999999"/>
+      </left>
+      <right style="hair">
+        <color rgb="FF999999"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF3465A4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair">
+        <color rgb="FF999999"/>
+      </left>
+      <right style="hair">
+        <color rgb="FF999999"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF3465A4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair">
+        <color rgb="FF999999"/>
+      </left>
+      <right style="hair">
+        <color rgb="FF999999"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF5B277D"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair">
+        <color rgb="FF999999"/>
+      </left>
+      <right style="hair">
+        <color rgb="FF999999"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF5B277D"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -287,21 +536,39 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -309,27 +576,161 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="12">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="column_head" xfId="20"/>
+    <cellStyle name="column_head_i18n" xfId="21"/>
+    <cellStyle name="group_begin" xfId="22"/>
+    <cellStyle name="group_end" xfId="23"/>
+    <cellStyle name="repeat_begin" xfId="24"/>
+    <cellStyle name="repeat_end" xfId="25"/>
   </cellStyles>
+  <dxfs count="5">
+    <dxf>
+      <border diagonalUp="false" diagonalDown="false">
+        <left style="hair">
+          <color rgb="FF999999"/>
+        </left>
+        <right style="hair">
+          <color rgb="FF999999"/>
+        </right>
+        <top style="medium">
+          <color rgb="FF3465A4"/>
+        </top>
+        <bottom/>
+        <diagonal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="false" diagonalDown="false">
+        <left style="hair">
+          <color rgb="FF999999"/>
+        </left>
+        <right style="hair">
+          <color rgb="FF999999"/>
+        </right>
+        <top/>
+        <bottom style="medium">
+          <color rgb="FF3465A4"/>
+        </bottom>
+        <diagonal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="false" diagonalDown="false">
+        <left style="hair">
+          <color rgb="FF999999"/>
+        </left>
+        <right style="hair">
+          <color rgb="FF999999"/>
+        </right>
+        <top style="medium">
+          <color rgb="FF5B277D"/>
+        </top>
+        <bottom/>
+        <diagonal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="false" diagonalDown="false">
+        <left style="hair">
+          <color rgb="FF999999"/>
+        </left>
+        <right style="hair">
+          <color rgb="FF999999"/>
+        </right>
+        <top/>
+        <bottom style="medium">
+          <color rgb="FF5B277D"/>
+        </bottom>
+        <diagonal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFCC0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFCCCCCC"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FFAFD095"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF3465A4"/>
+      <rgbColor rgb="FF999999"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF5B277D"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -444,250 +845,328 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:XFD21"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
+      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A30" activeCellId="0" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="90.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="58.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1010" min="5" style="1" width="14.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1015" min="1011" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16375" min="1016" style="1" width="14.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16376" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="37.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="56.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.28"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="30" style="1" width="11.53"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="1" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="1" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="1" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="1" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="1" t="s">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="XEV9" s="4"/>
-      <c r="XEW9" s="4"/>
-      <c r="XEX9" s="4"/>
-      <c r="XEY9" s="4"/>
-      <c r="XEZ9" s="4"/>
-      <c r="XFA9" s="4"/>
-      <c r="XFB9" s="4"/>
-      <c r="XFC9" s="4"/>
-      <c r="XFD9" s="4"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="1" t="s">
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1" t="s">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="1" t="s">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17" s="1" t="s">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="1" t="s">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>7</v>
+      <c r="B22" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="F2:G10000 A27:B27 A2:C26 A28:D10000 D2:D27">
+    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>$A2="begin_group"</formula>
+    </cfRule>
+    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>$A2="end_group"</formula>
+    </cfRule>
+    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>$A2="begin_repeat"</formula>
+    </cfRule>
+    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>$A2="end_repeat"</formula>
+    </cfRule>
+    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>AND(ISBLANK($A2), NOT(ISBLANK(A2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B10000">
+    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>AND(ISBLANK(B2), NOT(ISBLANK($A2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C28:C10000 C2:C26">
+    <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>AND(ISBLANK(C2),NOT(OR(ISBLANK($A2),$A2="calculate")))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C27">
+    <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>$A27="begin_group"</formula>
+    </cfRule>
+    <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>$A27="end_group"</formula>
+    </cfRule>
+    <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>$A27="begin_repeat"</formula>
+    </cfRule>
+    <cfRule type="expression" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>$A27="end_repeat"</formula>
+    </cfRule>
+    <cfRule type="expression" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>AND(ISBLANK($A27), NOT(ISBLANK(C27)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C27">
+    <cfRule type="expression" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>AND(ISBLANK(C27),NOT(OR(ISBLANK($A27),$A27="calculate")))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E10000">
+    <cfRule type="expression" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>$A2="begin_group"</formula>
+    </cfRule>
+    <cfRule type="expression" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>$A2="end_group"</formula>
+    </cfRule>
+    <cfRule type="expression" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>$A2="begin_repeat"</formula>
+    </cfRule>
+    <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>$A2="end_repeat"</formula>
+    </cfRule>
+    <cfRule type="expression" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>AND(ISBLANK($A2), NOT(ISBLANK(E2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E10000">
+    <cfRule type="expression" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>AND($A2="calculate", ISBLANK(E2))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation allowBlank="true" error="If configuring a select, ensure your list name matches a list from the choices sheet." errorStyle="information" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="A1" type="none">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" error="If configuring a select, ensure your list name matches a list from the choices sheet." errorStyle="information" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1015" type="list">
+      <formula1>"begin_group,end_group,note,calculate,text,integer,decimal,select_one list_name,select_multiple list_name,date,time,datetime,begin_repeat,end_repeat,geopoint,geotrace,geoshape,start-geopoint,range,image,audio,video,file,rank,acknowledge,start,end,today"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -696,70 +1175,63 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="1" width="17.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="7" style="1" width="17.29"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="21" style="5" width="14.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="17.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="20.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="16.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="32.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="2" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" s="6" t="str">
+        <f aca="true">TEXT(NOW(), "yyyymmddhhmmss")</f>
+        <v>20250213160007</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="7" t="n">
-        <f aca="true">TODAY()</f>
-        <v>45483</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>